<commit_message>
Added data analysis code for object files and time study
</commit_message>
<xml_diff>
--- a/RSVP_visual_now/Results/RSVP_spatial_cue_extended_letter_duration/RSVP_spatial_cue_extended_letter_durationsubject_level_stats.xlsx
+++ b/RSVP_visual_now/Results/RSVP_spatial_cue_extended_letter_duration/RSVP_spatial_cue_extended_letter_durationsubject_level_stats.xlsx
@@ -393,7 +393,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1036,6 +1036,35 @@
         <v>1</v>
       </c>
     </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
+        <v>22</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="D23" t="n">
+        <v>3.95</v>
+      </c>
+      <c r="E23" t="n">
+        <v>-0.11</v>
+      </c>
+      <c r="F23" t="n">
+        <v>4.34</v>
+      </c>
+      <c r="G23" t="n">
+        <v>-0.5289256198347108</v>
+      </c>
+      <c r="H23" t="n">
+        <v>-0.48</v>
+      </c>
+      <c r="I23" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>